<commit_message>
Update journal travail 09.02.2023
</commit_message>
<xml_diff>
--- a/Journal de travail.xlsx
+++ b/Journal de travail.xlsx
@@ -744,7 +744,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,13 +913,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>44963</v>
+        <v>44966</v>
       </c>
       <c r="B9" s="18">
         <v>1</v>
       </c>
       <c r="C9" s="11">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>6</v>
@@ -1051,7 +1051,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="1026" r:id="rId4" name="Button 2">
-              <controlPr defaultSize="0" autoFill="0" autoPict="0" macro="[0]!_xludf.Duplicate">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0" macro="[0]!Duplicate">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
@@ -1204,6 +1204,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B38552FA7D4254E8845977232CFE53B" ma:contentTypeVersion="7" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="03e14c2536b56bc7dd47f79481c7176c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0119da2b-60ce-4773-88fa-ebab2cde1f55" xmlns:ns3="c00db93e-a012-41a1-8dae-1f2fb8b40d56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b7050275a68257b53998f6363dd12a8" ns2:_="" ns3:_="">
     <xsd:import namespace="0119da2b-60ce-4773-88fa-ebab2cde1f55"/>
@@ -1386,22 +1401,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152F1D8-BC39-43C0-AFD5-9D59D80C8BCD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FF8A9A8-A00A-4ABC-BBD7-3D54D09AED55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c00db93e-a012-41a1-8dae-1f2fb8b40d56"/>
+    <ds:schemaRef ds:uri="0119da2b-60ce-4773-88fa-ebab2cde1f55"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD78DB3-3C09-4B83-8502-3F07A10F47B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1418,29 +1443,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FF8A9A8-A00A-4ABC-BBD7-3D54D09AED55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c00db93e-a012-41a1-8dae-1f2fb8b40d56"/>
-    <ds:schemaRef ds:uri="0119da2b-60ce-4773-88fa-ebab2cde1f55"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152F1D8-BC39-43C0-AFD5-9D59D80C8BCD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Create MCD and update planing
</commit_message>
<xml_diff>
--- a/Journal de travail.xlsx
+++ b/Journal de travail.xlsx
@@ -610,8 +610,8 @@
   <sheetPr codeName="Feuille1"/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,18 +1190,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1224,6 +1224,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152F1D8-BC39-43C0-AFD5-9D59D80C8BCD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FF8A9A8-A00A-4ABC-BBD7-3D54D09AED55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1238,12 +1246,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152F1D8-BC39-43C0-AFD5-9D59D80C8BCD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>